<commit_message>
first version, but need check
</commit_message>
<xml_diff>
--- a/dataset/data/Data_Dictionary.xlsx
+++ b/dataset/data/Data_Dictionary.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16060" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="train" sheetId="1" r:id="rId1"/>
@@ -12,9 +12,12 @@
     <sheet name="new_merchant_period" sheetId="4" r:id="rId3"/>
     <sheet name="merchant" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="157">
   <si>
     <t>train.csv</t>
   </si>
@@ -217,10 +220,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>卡id</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>一般是2018年3/4月，但也有最近没有交易的，就取的靠前，2017年的也有</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -405,10 +404,178 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <t>active_months_lag12</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>city_id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>state_id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>category_2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>month_lag</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>authorized_flag</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>category_3</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>category_1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>transaction和merchant中的category信息和city，state信息是通用的。并且category_1为Y时，没有category_2信息</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户对各类别交易次数及占比，交易过的类组数</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户对各类别交易次数及占比，交易过的类别数</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户交易过的商家数</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>category_4</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户对各商家组交易次数及占比，交易过的类别数</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户对各商家类别交易次数及占比，交易过的类别数</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户对各商家类组交易次数及占比，交易过的类别数</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>商家组id，109392个</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>商家类别id，325个</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>有效交易天数</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户每个month_lag交易次数及占比，最大最小差值</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>feature_1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>feature_2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>feature_3</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>first_active_month</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>merchant_group_id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>merchant_category_id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>subsector_id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>numerical_1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>avg_sales_lag3</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>avg_purchases_lag3</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>category_4</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>purchase_date</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>installments</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>subsector_id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户对各城市交易次数及占比</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>省份id，有-1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>商家类组id，42个，one-hot，有-1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>his_</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>his_</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>new_</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>purchase_amount</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>most_recent_sales_range</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <t>most_recent_purchases_range</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>active_months_lag3</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -417,179 +584,19 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>active_months_lag12</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>city_id</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>state_id</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>category_2</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>month_lag</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>authorized_flag</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>category_3</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>category_1</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>transaction和merchant中的category信息和city，state信息是通用的。并且category_1为Y时，没有category_2信息</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户对各类别交易次数及占比，交易过的类组数</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户对各类别交易次数及占比，交易过的类别数</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户交易过的商家数</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>category_4</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户对各商家组交易次数及占比，交易过的类别数</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户对各商家类别交易次数及占比，交易过的类别数</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户对各商家类组交易次数及占比，交易过的类别数</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>商家组id，109392个</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>商家类别id，325个</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>有效交易天数</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户每个month_lag交易次数及占比，最大最小差值</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>feature_1</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>feature_2</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>feature_3</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>first_active_month</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>merchant_group_id</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>merchant_category_id</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>subsector_id</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>numerical_1</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>most_recent_purchases_range</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>avg_sales_lag3</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>avg_purchases_lag3</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>category_4</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>purchase_date</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>installments</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>subsector_id</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>purchase_amount</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户对各城市交易次数及占比</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>省份id，有-1</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>商家类组id，42个，one-hot，有-1</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>his_</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>his_</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>new_</t>
+    <t>卡id,325541</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡id,290002</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -680,7 +687,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -722,9 +729,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A3:C9" totalsRowShown="0">
-  <autoFilter ref="A3:C9">
-    <filterColumn colId="2"/>
-  </autoFilter>
+  <autoFilter ref="A3:C9"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Columns"/>
     <tableColumn id="2" name="Description"/>
@@ -736,10 +741,7 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A3:D17" totalsRowShown="0">
-  <autoFilter ref="A3:D17">
-    <filterColumn colId="1"/>
-    <filterColumn colId="3"/>
-  </autoFilter>
+  <autoFilter ref="A3:D17"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Columns"/>
     <tableColumn id="4" name="重命名（前缀)" dataDxfId="2"/>
@@ -752,11 +754,7 @@
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela36" displayName="Tabela36" ref="A3:E17" totalsRowShown="0">
-  <autoFilter ref="A3:E17">
-    <filterColumn colId="1"/>
-    <filterColumn colId="3"/>
-    <filterColumn colId="4"/>
-  </autoFilter>
+  <autoFilter ref="A3:E17"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Columns"/>
     <tableColumn id="5" name="重命名（前缀)" dataDxfId="1"/>
@@ -770,11 +768,7 @@
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A3:E25" totalsRowShown="0">
-  <autoFilter ref="A3:E25">
-    <filterColumn colId="1"/>
-    <filterColumn colId="3"/>
-    <filterColumn colId="4"/>
-  </autoFilter>
+  <autoFilter ref="A3:E25"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Columns"/>
     <tableColumn id="5" name="重命名（前缀)" dataDxfId="0"/>
@@ -1041,25 +1035,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.25" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
     <col min="2" max="2" width="75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.875" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1076,7 +1070,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1089,7 +1083,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>53</v>
@@ -1097,35 +1091,35 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B6" t="s">
         <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B7" t="s">
         <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s">
         <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1142,27 +1136,32 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B17"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="46.875" customWidth="1"/>
-    <col min="4" max="4" width="32.375" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1177,7 +1176,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -1195,7 +1194,7 @@
         <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1203,13 +1202,13 @@
         <v>19</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C5" t="s">
         <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1221,7 +1220,7 @@
         <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1229,13 +1228,13 @@
         <v>56</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="4" customFormat="1">
@@ -1243,13 +1242,13 @@
         <v>57</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1257,13 +1256,13 @@
         <v>20</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1275,7 +1274,7 @@
         <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1287,7 +1286,7 @@
         <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1299,7 +1298,7 @@
         <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1307,13 +1306,13 @@
         <v>21</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C13" t="s">
         <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1321,13 +1320,13 @@
         <v>22</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1339,7 +1338,7 @@
         <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1351,7 +1350,7 @@
         <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1363,32 +1362,32 @@
         <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="C19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="C20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="C21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="C22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="C23" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1397,27 +1396,32 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="150" verticalDpi="150" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="150" verticalDpi="150"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="45.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.875" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" customWidth="1"/>
     <col min="5" max="5" width="34" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1438,7 +1442,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -1447,7 +1451,7 @@
         <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1459,130 +1463,130 @@
         <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C5" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" t="s">
         <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="8" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="6" customFormat="1">
       <c r="A11" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>49</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="6" customFormat="1">
       <c r="A12" s="6" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>50</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1590,73 +1594,73 @@
         <v>21</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C13" t="s">
         <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>149</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>155</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="6" customFormat="1">
       <c r="A15" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="6" customFormat="1">
       <c r="A16" s="6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>48</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1665,28 +1669,33 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="150" verticalDpi="150" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="150" verticalDpi="150"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.25" customWidth="1"/>
-    <col min="2" max="2" width="27.375" customWidth="1"/>
-    <col min="3" max="3" width="43.25" customWidth="1"/>
-    <col min="4" max="4" width="40.5" customWidth="1"/>
-    <col min="5" max="5" width="38.5" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" customWidth="1"/>
+    <col min="5" max="5" width="38.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1701,7 +1710,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -1710,7 +1719,7 @@
         <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1722,63 +1731,63 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" t="s">
         <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" t="s">
         <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" t="s">
         <v>46</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1789,29 +1798,29 @@
         <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="3" customFormat="1">
       <c r="A10" s="8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
-        <v>111</v>
+        <v>151</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>59</v>
@@ -1820,15 +1829,15 @@
         <v>61</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="7" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>60</v>
@@ -1837,38 +1846,38 @@
         <v>62</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="6" customFormat="1">
       <c r="A13" s="6" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="6" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" t="s">
         <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">
-        <v>112</v>
+        <v>153</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>7</v>
@@ -1877,10 +1886,10 @@
         <v>41</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1892,7 +1901,7 @@
         <v>29</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1904,12 +1913,12 @@
         <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="7" t="s">
-        <v>113</v>
+        <v>154</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>10</v>
@@ -1918,10 +1927,10 @@
         <v>42</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1933,7 +1942,7 @@
         <v>30</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1945,12 +1954,12 @@
         <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>13</v>
@@ -1959,32 +1968,32 @@
         <v>43</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="6" customFormat="1">
       <c r="A23" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>14</v>
@@ -1993,15 +2002,15 @@
         <v>47</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>15</v>
@@ -2010,27 +2019,27 @@
         <v>48</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="E24" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D25" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" t="s">
         <v>107</v>
-      </c>
-      <c r="E25" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2039,9 +2048,14 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="150" verticalDpi="150" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="150" verticalDpi="150"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>